<commit_message>
Fixed grid input file
</commit_message>
<xml_diff>
--- a/examples/create_scenario_with_grid/scenario_with_grid/agents.xlsx
+++ b/examples/create_scenario_with_grid/scenario_with_grid/agents.xlsx
@@ -736,19 +736,19 @@
     <t>pv/sizing/controllable_1</t>
   </si>
   <si>
-    <t>F2dVTofCrPU7TF2</t>
-  </si>
-  <si>
-    <t>hXavCOZVrRYFLa1</t>
-  </si>
-  <si>
-    <t>rccBZaDjv4mCtoq</t>
-  </si>
-  <si>
-    <t>pPrXmXwCXV1kEJY</t>
-  </si>
-  <si>
-    <t>UeLfzzzIvIGXlM5</t>
+    <t>Qy3FgxrlmWqen8U</t>
+  </si>
+  <si>
+    <t>PF0eMjEP47Ml37r</t>
+  </si>
+  <si>
+    <t>b8oa7IHrygg7DzW</t>
+  </si>
+  <si>
+    <t>PYDK5chfXHIU0Qe</t>
+  </si>
+  <si>
+    <t>Bg6ltWckoWhAk6i</t>
   </si>
   <si>
     <t>hh_2455_0.csv</t>
@@ -2393,10 +2393,10 @@
         <v>15385</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2405,7 +2405,7 @@
         <v>2.6</v>
       </c>
       <c r="J3">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2884,10 +2884,10 @@
         <v>17618</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -2896,7 +2896,7 @@
         <v>2.6</v>
       </c>
       <c r="J4">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>1</v>

</xml_diff>